<commit_message>
atualizando - tweets jornalisticos
</commit_message>
<xml_diff>
--- a/data/media_tweets_categorizada.xlsx
+++ b/data/media_tweets_categorizada.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,87 +412,87 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Conexão Política</t>
+          <t>Quebrando o tabu</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>direita; extrema-direita</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1433</v>
+        <v>10281</v>
       </c>
       <c r="E2">
-        <v>251</v>
+        <v>1280</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="G2">
-        <v>13</v>
+        <v>351</v>
       </c>
       <c r="H2">
-        <v>1433</v>
+        <v>2056</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Conexão Política</t>
+          <t>Quebrando o Tabu</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>conexaopolitica</t>
+          <t>QuebrandoOTabu</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Grupo Folha</t>
+          <t>Conexão Política</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>direita; centro-direita</t>
+          <t>direita; extrema-direita</t>
         </is>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>14669</v>
+        <v>1433</v>
       </c>
       <c r="E3">
-        <v>1034</v>
+        <v>251</v>
       </c>
       <c r="F3">
-        <v>2509</v>
+        <v>25</v>
       </c>
       <c r="G3">
-        <v>584</v>
+        <v>13</v>
       </c>
       <c r="H3">
-        <v>772</v>
+        <v>1433</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Folha de S.Paulo, UOL Notícias, UOL</t>
+          <t>Conexão Política</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>folha, UOLNoticias, UOL</t>
+          <t>conexaopolitica</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Grupo Globo</t>
+          <t>Grupo Folha</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -501,629 +501,709 @@
         </is>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>7103</v>
+        <v>14669</v>
       </c>
       <c r="E4">
-        <v>642</v>
+        <v>1034</v>
       </c>
       <c r="F4">
-        <v>671</v>
+        <v>2509</v>
       </c>
       <c r="G4">
-        <v>214</v>
+        <v>584</v>
       </c>
       <c r="H4">
-        <v>546</v>
+        <v>772</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Jornal O Globo, Jornal Extra, Lauro Jardim, Flávia Oliveira</t>
+          <t>Folha de S.Paulo, UOL Notícias, UOL</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>JornalOGlobo, jornalextra, laurojardim, flaviaol</t>
+          <t>folha, UOLNoticias, UOL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jornal da Cidade Online</t>
+          <t>Grupo Globo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>direita; extrema-direita</t>
+          <t>direita; centro-direita</t>
         </is>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>1567</v>
+        <v>7103</v>
       </c>
       <c r="E5">
-        <v>383</v>
+        <v>642</v>
       </c>
       <c r="F5">
-        <v>55</v>
+        <v>671</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="H5">
-        <v>522</v>
+        <v>546</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Jornal da Cidade Online</t>
+          <t>Jornal O Globo, Jornal Extra, Lauro Jardim, Flávia Oliveira</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>JornalDaCidadeO</t>
+          <t>JornalOGlobo, jornalextra, laurojardim, flaviaol</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Editora e Comercio Valongo</t>
+          <t>Jornal da Cidade Online</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>direita; centro-direita</t>
+          <t>direita; extrema-direita</t>
         </is>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>5876</v>
+        <v>1567</v>
       </c>
       <c r="E6">
-        <v>865</v>
+        <v>383</v>
       </c>
       <c r="F6">
-        <v>373</v>
+        <v>55</v>
       </c>
       <c r="G6">
-        <v>299</v>
+        <v>16</v>
       </c>
       <c r="H6">
-        <v>490</v>
+        <v>522</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>exame</t>
+          <t>Jornal da Cidade Online</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>exame</t>
+          <t>JornalDaCidadeO</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Oeste</t>
+          <t>Editora e Comercio Valongo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>direita</t>
+          <t>direita; centro-direita</t>
         </is>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>485</v>
+        <v>5876</v>
       </c>
       <c r="E7">
-        <v>89</v>
+        <v>865</v>
       </c>
       <c r="F7">
-        <v>80</v>
+        <v>373</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>299</v>
       </c>
       <c r="H7">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Revista Oeste</t>
+          <t>exame</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>revistaoeste</t>
+          <t>exame</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Publisher Brasil</t>
+          <t>Oeste</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>esquerda; centro-esquerda</t>
+          <t>direita</t>
         </is>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>2364</v>
+        <v>485</v>
       </c>
       <c r="E8">
-        <v>392</v>
+        <v>89</v>
       </c>
       <c r="F8">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H8">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Revista Fórum</t>
+          <t>Revista Oeste</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>revistaforum</t>
+          <t>revistaoeste</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Grupo Estado</t>
+          <t>Publisher Brasil</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>direita; centro-direita</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>2251</v>
+        <v>2364</v>
       </c>
       <c r="E9">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="F9">
-        <v>426</v>
+        <v>125</v>
       </c>
       <c r="G9">
-        <v>233</v>
+        <v>36</v>
       </c>
       <c r="H9">
-        <v>250</v>
+        <v>473</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Estadão 🗞️, Blog do Noblat</t>
+          <t>Revista Fórum</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Estadao, BlogdoNoblat</t>
+          <t>revistaforum</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Brasil 247</t>
+          <t>Grupo Estado</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>esquerda; centro-esquerda</t>
+          <t>direita; centro-direita</t>
         </is>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>1468</v>
+        <v>2251</v>
       </c>
       <c r="E10">
-        <v>273</v>
+        <v>383</v>
       </c>
       <c r="F10">
-        <v>54</v>
+        <v>426</v>
       </c>
       <c r="G10">
-        <v>29</v>
+        <v>233</v>
       </c>
       <c r="H10">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Brasil 247</t>
+          <t>Estadão 🗞️, Blog do Noblat</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>brasil247</t>
+          <t>Estadao, BlogdoNoblat</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Grupo Diario de Pernambuco; Diários Associados</t>
+          <t>Brasil 247</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>direita; centro-direita</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11">
-        <v>627</v>
+        <v>1468</v>
       </c>
       <c r="E11">
-        <v>17</v>
+        <v>273</v>
       </c>
       <c r="F11">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G11">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="H11">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Diario de Pernambuco</t>
+          <t>Brasil 247</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>DiarioPE</t>
+          <t>brasil247</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>British Broadcasting Corporation</t>
+          <t>Mídia NINJA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>centro</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>150</v>
+        <v>638</v>
       </c>
       <c r="E12">
-        <v>19</v>
+        <v>177</v>
       </c>
       <c r="F12">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="H12">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>BBC News Brasil</t>
+          <t>Mídia NINJA</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>bbcbrasil</t>
+          <t>MidiaNINJA</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Nn&amp;A Produções Jornalísticas</t>
+          <t>Grupo Diario de Pernambuco; Diários Associados</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>esquerda; centro-esquerda</t>
+          <t>direita; centro-direita</t>
         </is>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>891</v>
+        <v>627</v>
       </c>
       <c r="E13">
-        <v>219</v>
+        <v>17</v>
       </c>
       <c r="F13">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="G13">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H13">
-        <v>148</v>
+        <v>209</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>DCM ONLINE</t>
+          <t>Diario de Pernambuco</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>DCM_online</t>
+          <t>DiarioPE</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Grupo PRISA</t>
+          <t>British Broadcasting Corporation</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>esquerda; centro-esquerda</t>
+          <t>centro</t>
         </is>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E14">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H14">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>EL PAÍS Brasil</t>
+          <t>BBC News Brasil</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>elpais_brasil</t>
+          <t>bbcbrasil</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sistema Jornal do Commercio de Comunicação</t>
+          <t>Nn&amp;A Produções Jornalísticas</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>direita; centro-direita</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>792</v>
+        <v>891</v>
       </c>
       <c r="E15">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="F15">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="G15">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="H15">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Congresso em Foco, Jornal do Commercio</t>
+          <t>DCM ONLINE</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>congressoemfoco, jc_pe</t>
+          <t>DCM_online</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gazeta do Povo</t>
+          <t>Grupo PRISA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>direita; extrema-direita</t>
+          <t>esquerda; centro-esquerda</t>
         </is>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>359</v>
+        <v>140</v>
       </c>
       <c r="E16">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="F16">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
       <c r="H16">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Gazeta do Povo, Madeleine Lacsko</t>
+          <t>EL PAÍS Brasil</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>gazetadopovo, madeleinelacsko</t>
+          <t>elpais_brasil</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CNN Brasil Novus Mídia</t>
+          <t>Sistema Jornal do Commercio de Comunicação</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>direita</t>
+          <t>direita; centro-direita</t>
         </is>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>622</v>
+        <v>792</v>
       </c>
       <c r="E17">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="F17">
-        <v>179</v>
+        <v>63</v>
       </c>
       <c r="G17">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H17">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>CNN Brasil Business</t>
+          <t>Congresso em Foco, Jornal do Commercio</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>CNNBrBusiness</t>
+          <t>congressoemfoco, jc_pe</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Grupo Metrópoles</t>
+          <t>Gazeta do Povo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>esquerda; centro-esquerda</t>
+          <t>direita; extrema-direita</t>
         </is>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="E18">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F18">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="G18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Metrópoles</t>
+          <t>Gazeta do Povo, Madeleine Lacsko</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Metropoles</t>
+          <t>gazetadopovo, madeleinelacsko</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>CNN Brasil Novus Mídia</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>direita</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>622</v>
+      </c>
+      <c r="E19">
+        <v>74</v>
+      </c>
+      <c r="F19">
+        <v>179</v>
+      </c>
+      <c r="G19">
+        <v>150</v>
+      </c>
+      <c r="H19">
+        <v>69</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>CNN Brasil Business</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CNNBrBusiness</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Grupo Metrópoles</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>esquerda; centro-esquerda</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>332</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20">
+        <v>36</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>66</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Metrópoles</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Metropoles</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>Diários Associados</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>direita; centro-direita</t>
         </is>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>11</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>448</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>44</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <v>69</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>27</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>41</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Correio Braziliense, Estado de Minas</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>correio, em_com</t>
         </is>

</xml_diff>